<commit_message>
little updates & added igs
</commit_message>
<xml_diff>
--- a/Drawings/CARRIAGE_BOM.xlsx
+++ b/Drawings/CARRIAGE_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\GitHub\SpindleCarriageForCNC\Drawings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5437CE12-3CCD-40BF-BD71-4FF7AF1862FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A5F1E0-9EA7-4499-8E18-0FA98577C979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,16 +23,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'arrangement-mat'!$A$1:$M$73</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -148,9 +138,6 @@
   </si>
   <si>
     <t>2</t>
-  </si>
-  <si>
-    <t>Corner Bracket 40х40L</t>
   </si>
   <si>
     <t>AISI 1035 Steel (SS)</t>
@@ -581,6 +568,9 @@
   </si>
   <si>
     <t>91166A240</t>
+  </si>
+  <si>
+    <t>Corner Bracket 40х20L</t>
   </si>
 </sst>
 </file>
@@ -1764,116 +1754,116 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2450,8 +2440,8 @@
   <dimension ref="A1:Q293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R59" sqref="R59"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2572,8 +2562,8 @@
         <v>CARRIAGE_BOM.xlsx</v>
       </c>
       <c r="H5" s="174"/>
-      <c r="I5" s="187"/>
-      <c r="J5" s="187"/>
+      <c r="I5" s="214"/>
+      <c r="J5" s="214"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="17"/>
@@ -2589,7 +2579,7 @@
       </c>
       <c r="G6" s="22">
         <f ca="1">TODAY()</f>
-        <v>44926</v>
+        <v>44941</v>
       </c>
       <c r="H6" s="21" t="s">
         <v>5</v>
@@ -2610,10 +2600,10 @@
       <c r="C7" s="166" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="185" t="s">
+      <c r="D7" s="212" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="186"/>
+      <c r="E7" s="213"/>
       <c r="F7" s="168" t="s">
         <v>4</v>
       </c>
@@ -2636,7 +2626,7 @@
         <v>30</v>
       </c>
       <c r="M7" s="172" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N7" s="26" t="s">
         <v>33</v>
@@ -2650,26 +2640,26 @@
     </row>
     <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="188" t="s">
-        <v>96</v>
+      <c r="B8" s="182" t="s">
+        <v>95</v>
       </c>
       <c r="C8" s="28"/>
-      <c r="D8" s="191">
+      <c r="D8" s="210">
         <v>2</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="30"/>
       <c r="G8" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H8" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="31" t="s">
         <v>97</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>98</v>
       </c>
       <c r="K8" s="32" t="s">
         <v>31</v>
@@ -2684,9 +2674,9 @@
     </row>
     <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="189"/>
+      <c r="B9" s="183"/>
       <c r="C9" s="34"/>
-      <c r="D9" s="192"/>
+      <c r="D9" s="215"/>
       <c r="E9" s="35"/>
       <c r="F9" s="36"/>
       <c r="G9" s="37"/>
@@ -2695,7 +2685,7 @@
         <v>31</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K9" s="40" t="s">
         <v>31</v>
@@ -2705,52 +2695,52 @@
     </row>
     <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="190"/>
+      <c r="B10" s="209"/>
       <c r="C10" s="53"/>
-      <c r="D10" s="193"/>
+      <c r="D10" s="211"/>
       <c r="E10" s="104"/>
       <c r="F10" s="127"/>
       <c r="G10" s="127"/>
       <c r="H10" s="127"/>
       <c r="I10" s="58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J10" s="58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K10" s="153" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L10" s="149"/>
       <c r="M10" s="60"/>
     </row>
     <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11" s="179" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="181" t="s">
+      <c r="B11" s="184" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="183">
+      <c r="D11" s="194">
         <v>1</v>
       </c>
       <c r="E11" s="103"/>
       <c r="F11" s="45"/>
       <c r="G11" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H11" s="103" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I11" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K11" s="47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L11" s="147">
         <v>62.17</v>
@@ -2762,13 +2752,13 @@
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="180"/>
-      <c r="C12" s="182"/>
-      <c r="D12" s="184"/>
+      <c r="B12" s="185"/>
+      <c r="C12" s="187"/>
+      <c r="D12" s="195"/>
       <c r="E12" s="104"/>
       <c r="F12" s="49"/>
       <c r="G12" s="50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H12" s="51"/>
       <c r="I12" s="51"/>
@@ -2779,11 +2769,11 @@
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="188" t="s">
+      <c r="B13" s="182" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="28"/>
-      <c r="D13" s="191">
+      <c r="D13" s="210">
         <v>1</v>
       </c>
       <c r="E13" s="29"/>
@@ -2792,7 +2782,7 @@
         <v>24</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I13" s="31" t="s">
         <v>31</v>
@@ -2813,13 +2803,13 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="190"/>
+      <c r="B14" s="209"/>
       <c r="C14" s="53"/>
-      <c r="D14" s="193"/>
+      <c r="D14" s="211"/>
       <c r="E14" s="54"/>
       <c r="F14" s="55"/>
       <c r="G14" s="56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H14" s="57"/>
       <c r="I14" s="58"/>
@@ -2830,11 +2820,11 @@
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="194" t="s">
+      <c r="B15" s="203" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="61"/>
-      <c r="D15" s="198">
+      <c r="D15" s="207">
         <v>1</v>
       </c>
       <c r="E15" s="103"/>
@@ -2843,7 +2833,7 @@
         <v>25</v>
       </c>
       <c r="H15" s="103" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I15" s="46" t="s">
         <v>31</v>
@@ -2864,13 +2854,13 @@
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="195"/>
+      <c r="B16" s="204"/>
       <c r="C16" s="65"/>
-      <c r="D16" s="199"/>
+      <c r="D16" s="208"/>
       <c r="E16" s="104"/>
       <c r="F16" s="66"/>
       <c r="G16" s="67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H16" s="68"/>
       <c r="I16" s="51"/>
@@ -2882,7 +2872,7 @@
     <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="71"/>
       <c r="D17" s="72">
@@ -2891,16 +2881,16 @@
       <c r="E17" s="72"/>
       <c r="F17" s="73"/>
       <c r="G17" s="74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H17" s="72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I17" s="74" t="s">
         <v>31</v>
       </c>
       <c r="J17" s="74" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K17" s="106" t="s">
         <v>31</v>
@@ -2916,7 +2906,7 @@
     <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="77"/>
       <c r="D18" s="78">
@@ -2925,16 +2915,16 @@
       <c r="E18" s="78"/>
       <c r="F18" s="79"/>
       <c r="G18" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="H18" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="H18" s="78" t="s">
+      <c r="I18" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="80" t="s">
         <v>109</v>
-      </c>
-      <c r="I18" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="J18" s="80" t="s">
-        <v>110</v>
       </c>
       <c r="K18" s="154" t="s">
         <v>31</v>
@@ -2950,7 +2940,7 @@
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" s="71"/>
       <c r="D19" s="72">
@@ -2959,19 +2949,19 @@
       <c r="E19" s="72"/>
       <c r="F19" s="73"/>
       <c r="G19" s="74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H19" s="72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I19" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K19" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L19" s="150">
         <v>0.48</v>
@@ -2985,7 +2975,7 @@
     <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="76" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="77"/>
       <c r="D20" s="78">
@@ -2994,16 +2984,16 @@
       <c r="E20" s="78"/>
       <c r="F20" s="79"/>
       <c r="G20" s="80" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="80" t="s">
         <v>114</v>
-      </c>
-      <c r="H20" s="78" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="J20" s="80" t="s">
-        <v>115</v>
       </c>
       <c r="K20" s="154" t="s">
         <v>31</v>
@@ -3019,7 +3009,7 @@
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="71"/>
       <c r="D21" s="72">
@@ -3028,19 +3018,19 @@
       <c r="E21" s="72"/>
       <c r="F21" s="73"/>
       <c r="G21" s="74" t="s">
+        <v>153</v>
+      </c>
+      <c r="H21" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="72" t="s">
-        <v>38</v>
-      </c>
       <c r="I21" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="J21" s="74" t="s">
-        <v>52</v>
-      </c>
       <c r="K21" s="106" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L21" s="150">
         <v>49</v>
@@ -3053,7 +3043,7 @@
     <row r="22" spans="1:17" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="84"/>
       <c r="B22" s="76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="77"/>
       <c r="D22" s="78">
@@ -3062,19 +3052,19 @@
       <c r="E22" s="78"/>
       <c r="F22" s="79"/>
       <c r="G22" s="80" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H22" s="78" t="s">
         <v>27</v>
       </c>
       <c r="I22" s="80" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J22" s="80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K22" s="85" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L22" s="152">
         <v>25</v>
@@ -3087,7 +3077,7 @@
     <row r="23" spans="1:17" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="84"/>
       <c r="B23" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="71"/>
       <c r="D23" s="72">
@@ -3096,19 +3086,19 @@
       <c r="E23" s="72"/>
       <c r="F23" s="73"/>
       <c r="G23" s="74" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H23" s="72" t="s">
         <v>27</v>
       </c>
       <c r="I23" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K23" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L23" s="150">
         <v>37</v>
@@ -3120,7 +3110,7 @@
     </row>
     <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="77"/>
       <c r="D24" s="78">
@@ -3129,19 +3119,19 @@
       <c r="E24" s="78"/>
       <c r="F24" s="79"/>
       <c r="G24" s="80" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H24" s="78" t="s">
         <v>27</v>
       </c>
       <c r="I24" s="80" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J24" s="80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K24" s="85" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L24" s="152">
         <v>1.6</v>
@@ -3155,7 +3145,7 @@
     <row r="25" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="87"/>
       <c r="B25" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="71"/>
       <c r="D25" s="72">
@@ -3164,19 +3154,19 @@
       <c r="E25" s="72"/>
       <c r="F25" s="73"/>
       <c r="G25" s="74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H25" s="72" t="s">
         <v>27</v>
       </c>
       <c r="I25" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J25" s="74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K25" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L25" s="150">
         <v>315</v>
@@ -3192,7 +3182,7 @@
     <row r="26" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="87"/>
       <c r="B26" s="76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="77"/>
       <c r="D26" s="78">
@@ -3201,16 +3191,16 @@
       <c r="E26" s="78"/>
       <c r="F26" s="79"/>
       <c r="G26" s="80" t="s">
+        <v>117</v>
+      </c>
+      <c r="H26" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="H26" s="78" t="s">
+      <c r="I26" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="80" t="s">
         <v>119</v>
-      </c>
-      <c r="I26" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="J26" s="80" t="s">
-        <v>120</v>
       </c>
       <c r="K26" s="154" t="s">
         <v>31</v>
@@ -3229,7 +3219,7 @@
     <row r="27" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="87"/>
       <c r="B27" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="71"/>
       <c r="D27" s="72">
@@ -3238,19 +3228,19 @@
       <c r="E27" s="72"/>
       <c r="F27" s="73"/>
       <c r="G27" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="H27" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="H27" s="72" t="s">
-        <v>122</v>
-      </c>
       <c r="I27" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J27" s="74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K27" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L27" s="150">
         <v>1.34</v>
@@ -3265,7 +3255,7 @@
     </row>
     <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="77"/>
       <c r="D28" s="78">
@@ -3274,16 +3264,16 @@
       <c r="E28" s="78"/>
       <c r="F28" s="79"/>
       <c r="G28" s="80" t="s">
+        <v>122</v>
+      </c>
+      <c r="H28" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="I28" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" s="80" t="s">
         <v>123</v>
-      </c>
-      <c r="H28" s="78" t="s">
-        <v>122</v>
-      </c>
-      <c r="I28" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="J28" s="80" t="s">
-        <v>124</v>
       </c>
       <c r="K28" s="154" t="s">
         <v>31</v>
@@ -3298,7 +3288,7 @@
     </row>
     <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="71"/>
       <c r="D29" s="72">
@@ -3307,16 +3297,16 @@
       <c r="E29" s="72"/>
       <c r="F29" s="73"/>
       <c r="G29" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="H29" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="H29" s="72" t="s">
+      <c r="I29" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29" s="74" t="s">
         <v>126</v>
-      </c>
-      <c r="I29" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="J29" s="74" t="s">
-        <v>127</v>
       </c>
       <c r="K29" s="106" t="s">
         <v>31</v>
@@ -3332,7 +3322,7 @@
     <row r="30" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="87"/>
       <c r="B30" s="76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="77"/>
       <c r="D30" s="78">
@@ -3341,19 +3331,19 @@
       <c r="E30" s="78"/>
       <c r="F30" s="79"/>
       <c r="G30" s="80" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H30" s="78" t="s">
         <v>27</v>
       </c>
       <c r="I30" s="80" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J30" s="80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K30" s="85" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L30" s="152">
         <v>314</v>
@@ -3368,7 +3358,7 @@
     </row>
     <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="71"/>
       <c r="D31" s="72">
@@ -3377,19 +3367,19 @@
       <c r="E31" s="72"/>
       <c r="F31" s="73"/>
       <c r="G31" s="74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H31" s="72" t="s">
         <v>27</v>
       </c>
       <c r="I31" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J31" s="74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K31" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L31" s="150">
         <v>5.1100000000000003</v>
@@ -3402,7 +3392,7 @@
     <row r="32" spans="1:17" s="91" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="90"/>
       <c r="B32" s="76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="77"/>
       <c r="D32" s="78">
@@ -3411,19 +3401,19 @@
       <c r="E32" s="78"/>
       <c r="F32" s="79"/>
       <c r="G32" s="80" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H32" s="78" t="s">
         <v>27</v>
       </c>
       <c r="I32" s="80" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J32" s="80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K32" s="85" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L32" s="152">
         <v>49</v>
@@ -3437,7 +3427,7 @@
     <row r="33" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="84"/>
       <c r="B33" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="71"/>
       <c r="D33" s="72">
@@ -3446,19 +3436,19 @@
       <c r="E33" s="72"/>
       <c r="F33" s="73"/>
       <c r="G33" s="74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H33" s="72" t="s">
         <v>27</v>
       </c>
       <c r="I33" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J33" s="74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K33" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L33" s="150">
         <v>10</v>
@@ -3474,7 +3464,7 @@
     <row r="34" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="77"/>
       <c r="D34" s="78">
@@ -3483,19 +3473,19 @@
       <c r="E34" s="78"/>
       <c r="F34" s="79"/>
       <c r="G34" s="80" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H34" s="78" t="s">
         <v>27</v>
       </c>
       <c r="I34" s="80" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J34" s="80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K34" s="85" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L34" s="152">
         <v>16</v>
@@ -3511,7 +3501,7 @@
     <row r="35" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="90"/>
       <c r="B35" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="71"/>
       <c r="D35" s="72">
@@ -3520,7 +3510,7 @@
       <c r="E35" s="72"/>
       <c r="F35" s="73"/>
       <c r="G35" s="74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H35" s="72" t="s">
         <v>27</v>
@@ -3529,7 +3519,7 @@
         <v>31</v>
       </c>
       <c r="J35" s="74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K35" s="106" t="s">
         <v>31</v>
@@ -3548,7 +3538,7 @@
     <row r="36" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" s="77"/>
       <c r="D36" s="78">
@@ -3557,7 +3547,7 @@
       <c r="E36" s="78"/>
       <c r="F36" s="79"/>
       <c r="G36" s="80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H36" s="78" t="s">
         <v>27</v>
@@ -3566,7 +3556,7 @@
         <v>31</v>
       </c>
       <c r="J36" s="80" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K36" s="154" t="s">
         <v>31</v>
@@ -3585,7 +3575,7 @@
     <row r="37" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="87"/>
       <c r="B37" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="71"/>
       <c r="D37" s="72">
@@ -3594,19 +3584,19 @@
       <c r="E37" s="72"/>
       <c r="F37" s="73"/>
       <c r="G37" s="74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H37" s="72" t="s">
         <v>27</v>
       </c>
       <c r="I37" s="74" t="s">
+        <v>136</v>
+      </c>
+      <c r="J37" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="82" t="s">
         <v>137</v>
-      </c>
-      <c r="J37" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="K37" s="82" t="s">
-        <v>138</v>
       </c>
       <c r="L37" s="150">
         <v>1</v>
@@ -3621,31 +3611,31 @@
     </row>
     <row r="38" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="194" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="196" t="s">
+      <c r="B38" s="203" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="205" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="198">
+      <c r="D38" s="207">
         <v>1</v>
       </c>
       <c r="E38" s="103"/>
       <c r="F38" s="62"/>
       <c r="G38" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="H38" s="103" t="s">
         <v>139</v>
       </c>
-      <c r="H38" s="103" t="s">
-        <v>140</v>
-      </c>
       <c r="I38" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J38" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K38" s="47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L38" s="147">
         <v>11.5</v>
@@ -3660,13 +3650,13 @@
     </row>
     <row r="39" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="195"/>
-      <c r="C39" s="197"/>
-      <c r="D39" s="199"/>
+      <c r="B39" s="204"/>
+      <c r="C39" s="206"/>
+      <c r="D39" s="208"/>
       <c r="E39" s="104"/>
       <c r="F39" s="51"/>
       <c r="G39" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H39" s="104"/>
       <c r="I39" s="51"/>
@@ -3690,7 +3680,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="160" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L40" s="163"/>
       <c r="M40" s="162">
@@ -3704,7 +3694,7 @@
     <row r="41" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="107" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="3"/>
@@ -3723,26 +3713,26 @@
     </row>
     <row r="42" spans="1:17" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
-      <c r="B42" s="188" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="205"/>
-      <c r="D42" s="200">
+      <c r="B42" s="182" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="199"/>
+      <c r="D42" s="192">
         <v>1</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="126"/>
       <c r="G42" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H42" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I42" s="31" t="s">
         <v>31</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K42" s="102" t="s">
         <v>31</v>
@@ -3759,13 +3749,13 @@
       <c r="Q42" s="89"/>
     </row>
     <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="189"/>
-      <c r="C43" s="206"/>
-      <c r="D43" s="201"/>
+      <c r="B43" s="183"/>
+      <c r="C43" s="200"/>
+      <c r="D43" s="193"/>
       <c r="E43" s="155"/>
       <c r="F43" s="156"/>
       <c r="G43" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H43" s="157"/>
       <c r="I43" s="43"/>
@@ -3775,26 +3765,26 @@
       <c r="M43" s="44"/>
     </row>
     <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="179" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="181"/>
-      <c r="D44" s="183">
+      <c r="B44" s="184" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="186"/>
+      <c r="D44" s="194">
         <v>1</v>
       </c>
       <c r="E44" s="103"/>
       <c r="F44" s="129"/>
       <c r="G44" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H44" s="103" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I44" s="46" t="s">
         <v>31</v>
       </c>
       <c r="J44" s="46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K44" s="130" t="s">
         <v>31</v>
@@ -3808,13 +3798,13 @@
       </c>
     </row>
     <row r="45" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="180"/>
-      <c r="C45" s="182"/>
-      <c r="D45" s="184"/>
+      <c r="B45" s="185"/>
+      <c r="C45" s="187"/>
+      <c r="D45" s="195"/>
       <c r="E45" s="104"/>
       <c r="F45" s="131"/>
       <c r="G45" s="132" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H45" s="68"/>
       <c r="I45" s="51"/>
@@ -3824,26 +3814,26 @@
       <c r="M45" s="52"/>
     </row>
     <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="213" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="211"/>
-      <c r="D46" s="200">
+      <c r="B46" s="190" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="188"/>
+      <c r="D46" s="192">
         <v>2</v>
       </c>
       <c r="E46" s="29"/>
       <c r="F46" s="126"/>
       <c r="G46" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H46" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I46" s="31" t="s">
         <v>31</v>
       </c>
       <c r="J46" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K46" s="134" t="s">
         <v>31</v>
@@ -3857,13 +3847,13 @@
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="214"/>
-      <c r="C47" s="212"/>
-      <c r="D47" s="202"/>
+      <c r="B47" s="191"/>
+      <c r="C47" s="189"/>
+      <c r="D47" s="196"/>
       <c r="E47" s="54"/>
       <c r="F47" s="120"/>
       <c r="G47" s="127" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H47" s="57"/>
       <c r="I47" s="58"/>
@@ -3873,26 +3863,26 @@
       <c r="M47" s="60"/>
     </row>
     <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="209" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="207"/>
-      <c r="D48" s="203">
+      <c r="B48" s="180" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="201"/>
+      <c r="D48" s="197">
         <v>1</v>
       </c>
       <c r="E48" s="135"/>
       <c r="F48" s="136"/>
       <c r="G48" s="137" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H48" s="135" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I48" s="137" t="s">
         <v>31</v>
       </c>
       <c r="J48" s="137" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K48" s="138" t="s">
         <v>31</v>
@@ -3906,13 +3896,13 @@
       </c>
     </row>
     <row r="49" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="210"/>
-      <c r="C49" s="208"/>
-      <c r="D49" s="204"/>
+      <c r="B49" s="181"/>
+      <c r="C49" s="202"/>
+      <c r="D49" s="198"/>
       <c r="E49" s="139"/>
       <c r="F49" s="140"/>
       <c r="G49" s="141" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H49" s="142"/>
       <c r="I49" s="143"/>
@@ -3923,7 +3913,7 @@
     </row>
     <row r="50" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K50" s="160" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L50" s="161"/>
       <c r="M50" s="162">
@@ -3947,7 +3937,7 @@
     </row>
     <row r="52" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" s="108"/>
       <c r="D52" s="72">
@@ -3956,19 +3946,19 @@
       <c r="E52" s="72"/>
       <c r="F52" s="109"/>
       <c r="G52" s="109" t="s">
+        <v>67</v>
+      </c>
+      <c r="H52" s="110" t="s">
+        <v>48</v>
+      </c>
+      <c r="I52" s="109" t="s">
+        <v>66</v>
+      </c>
+      <c r="J52" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="H52" s="110" t="s">
-        <v>49</v>
-      </c>
-      <c r="I52" s="109" t="s">
-        <v>67</v>
-      </c>
-      <c r="J52" s="109" t="s">
-        <v>69</v>
-      </c>
       <c r="K52" s="111" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L52" s="150">
         <v>0.23</v>
@@ -3980,7 +3970,7 @@
     </row>
     <row r="53" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="113"/>
       <c r="D53" s="114">
@@ -3989,19 +3979,19 @@
       <c r="E53" s="114"/>
       <c r="F53" s="115"/>
       <c r="G53" s="115" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H53" s="116" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I53" s="115" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J53" s="115" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K53" s="117" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L53" s="159">
         <v>0.65</v>
@@ -4013,7 +4003,7 @@
     </row>
     <row r="54" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="108"/>
       <c r="D54" s="72">
@@ -4022,16 +4012,16 @@
       <c r="E54" s="72"/>
       <c r="F54" s="109"/>
       <c r="G54" s="109" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H54" s="110" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I54" s="109" t="s">
         <v>31</v>
       </c>
       <c r="J54" s="109" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K54" s="111" t="s">
         <v>31</v>
@@ -4046,7 +4036,7 @@
     </row>
     <row r="55" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" s="113"/>
       <c r="D55" s="114">
@@ -4055,16 +4045,16 @@
       <c r="E55" s="114"/>
       <c r="F55" s="115"/>
       <c r="G55" s="115" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H55" s="116" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I55" s="115" t="s">
         <v>31</v>
       </c>
       <c r="J55" s="115" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K55" s="117" t="s">
         <v>31</v>
@@ -4079,7 +4069,7 @@
     </row>
     <row r="56" spans="2:13" ht="15" x14ac:dyDescent="0.2">
       <c r="B56" s="98" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="99"/>
       <c r="D56" s="29">
@@ -4088,19 +4078,19 @@
       <c r="E56" s="29"/>
       <c r="F56" s="100"/>
       <c r="G56" s="100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H56" s="101" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I56" s="100" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J56" s="100" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K56" s="102" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L56" s="145">
         <v>3.63</v>
@@ -4122,7 +4112,7 @@
         <v>31</v>
       </c>
       <c r="J57" s="120" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K57" s="121" t="s">
         <v>31</v>
@@ -4132,7 +4122,7 @@
     </row>
     <row r="58" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="113"/>
       <c r="D58" s="114">
@@ -4141,16 +4131,16 @@
       <c r="E58" s="114"/>
       <c r="F58" s="115"/>
       <c r="G58" s="115" t="s">
+        <v>71</v>
+      </c>
+      <c r="H58" s="116" t="s">
+        <v>49</v>
+      </c>
+      <c r="I58" s="115" t="s">
+        <v>31</v>
+      </c>
+      <c r="J58" s="115" t="s">
         <v>72</v>
-      </c>
-      <c r="H58" s="116" t="s">
-        <v>50</v>
-      </c>
-      <c r="I58" s="115" t="s">
-        <v>31</v>
-      </c>
-      <c r="J58" s="115" t="s">
-        <v>73</v>
       </c>
       <c r="K58" s="117" t="s">
         <v>31</v>
@@ -4165,7 +4155,7 @@
     </row>
     <row r="59" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" s="108"/>
       <c r="D59" s="72">
@@ -4174,16 +4164,16 @@
       <c r="E59" s="72"/>
       <c r="F59" s="109"/>
       <c r="G59" s="109" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H59" s="110" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I59" s="109" t="s">
         <v>31</v>
       </c>
       <c r="J59" s="109" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K59" s="111" t="s">
         <v>31</v>
@@ -4198,7 +4188,7 @@
     </row>
     <row r="60" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B60" s="112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" s="113"/>
       <c r="D60" s="114">
@@ -4207,16 +4197,16 @@
       <c r="E60" s="114"/>
       <c r="F60" s="115"/>
       <c r="G60" s="115" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H60" s="116" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I60" s="115" t="s">
         <v>31</v>
       </c>
       <c r="J60" s="115" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K60" s="117" t="s">
         <v>31</v>
@@ -4231,7 +4221,7 @@
     </row>
     <row r="61" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B61" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C61" s="108"/>
       <c r="D61" s="72">
@@ -4240,16 +4230,16 @@
       <c r="E61" s="72"/>
       <c r="F61" s="109"/>
       <c r="G61" s="109" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H61" s="110" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I61" s="109" t="s">
         <v>31</v>
       </c>
       <c r="J61" s="109" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K61" s="111" t="s">
         <v>31</v>
@@ -4264,7 +4254,7 @@
     </row>
     <row r="62" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B62" s="112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" s="113"/>
       <c r="D62" s="114">
@@ -4273,18 +4263,18 @@
       <c r="E62" s="114"/>
       <c r="F62" s="115"/>
       <c r="G62" s="115" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H62" s="116" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I62" s="115" t="s">
         <v>31</v>
       </c>
       <c r="J62" s="115" t="s">
-        <v>153</v>
-      </c>
-      <c r="K62" s="215" t="s">
+        <v>152</v>
+      </c>
+      <c r="K62" s="179" t="s">
         <v>31</v>
       </c>
       <c r="L62" s="159">
@@ -4297,7 +4287,7 @@
     </row>
     <row r="63" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63" s="108"/>
       <c r="D63" s="72">
@@ -4306,16 +4296,16 @@
       <c r="E63" s="72"/>
       <c r="F63" s="109"/>
       <c r="G63" s="109" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H63" s="110" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I63" s="109" t="s">
         <v>31</v>
       </c>
       <c r="J63" s="109" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K63" s="111" t="s">
         <v>31</v>
@@ -4330,7 +4320,7 @@
     </row>
     <row r="64" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C64" s="113"/>
       <c r="D64" s="114">
@@ -4339,16 +4329,16 @@
       <c r="E64" s="114"/>
       <c r="F64" s="115"/>
       <c r="G64" s="115" t="s">
+        <v>77</v>
+      </c>
+      <c r="H64" s="116" t="s">
+        <v>76</v>
+      </c>
+      <c r="I64" s="115" t="s">
+        <v>31</v>
+      </c>
+      <c r="J64" s="115" t="s">
         <v>78</v>
-      </c>
-      <c r="H64" s="116" t="s">
-        <v>77</v>
-      </c>
-      <c r="I64" s="115" t="s">
-        <v>31</v>
-      </c>
-      <c r="J64" s="115" t="s">
-        <v>79</v>
       </c>
       <c r="K64" s="117" t="s">
         <v>31</v>
@@ -4363,7 +4353,7 @@
     </row>
     <row r="65" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B65" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C65" s="108"/>
       <c r="D65" s="72">
@@ -4372,16 +4362,16 @@
       <c r="E65" s="72"/>
       <c r="F65" s="109"/>
       <c r="G65" s="109" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H65" s="110" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I65" s="109" t="s">
         <v>31</v>
       </c>
       <c r="J65" s="109" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K65" s="111" t="s">
         <v>31</v>
@@ -4396,7 +4386,7 @@
     </row>
     <row r="66" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B66" s="112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66" s="113"/>
       <c r="D66" s="114">
@@ -4405,16 +4395,16 @@
       <c r="E66" s="114"/>
       <c r="F66" s="115"/>
       <c r="G66" s="115" t="s">
+        <v>80</v>
+      </c>
+      <c r="H66" s="116" t="s">
         <v>81</v>
       </c>
-      <c r="H66" s="116" t="s">
+      <c r="I66" s="115" t="s">
+        <v>31</v>
+      </c>
+      <c r="J66" s="115" t="s">
         <v>82</v>
-      </c>
-      <c r="I66" s="115" t="s">
-        <v>31</v>
-      </c>
-      <c r="J66" s="115" t="s">
-        <v>83</v>
       </c>
       <c r="K66" s="117" t="s">
         <v>31</v>
@@ -4429,7 +4419,7 @@
     </row>
     <row r="67" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C67" s="108"/>
       <c r="D67" s="72">
@@ -4438,16 +4428,16 @@
       <c r="E67" s="72"/>
       <c r="F67" s="109"/>
       <c r="G67" s="109" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H67" s="110" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I67" s="109" t="s">
         <v>31</v>
       </c>
       <c r="J67" s="109" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K67" s="111" t="s">
         <v>31</v>
@@ -4462,7 +4452,7 @@
     </row>
     <row r="68" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B68" s="112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C68" s="116"/>
       <c r="D68" s="114">
@@ -4471,16 +4461,16 @@
       <c r="E68" s="114"/>
       <c r="F68" s="122"/>
       <c r="G68" s="122" t="s">
+        <v>84</v>
+      </c>
+      <c r="H68" s="116" t="s">
+        <v>49</v>
+      </c>
+      <c r="I68" s="115" t="s">
+        <v>31</v>
+      </c>
+      <c r="J68" s="122" t="s">
         <v>85</v>
-      </c>
-      <c r="H68" s="116" t="s">
-        <v>50</v>
-      </c>
-      <c r="I68" s="115" t="s">
-        <v>31</v>
-      </c>
-      <c r="J68" s="122" t="s">
-        <v>86</v>
       </c>
       <c r="K68" s="117" t="s">
         <v>31</v>
@@ -4495,7 +4485,7 @@
     </row>
     <row r="69" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B69" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C69" s="110"/>
       <c r="D69" s="72">
@@ -4504,16 +4494,16 @@
       <c r="E69" s="72"/>
       <c r="F69" s="74"/>
       <c r="G69" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="H69" s="110" t="s">
+        <v>49</v>
+      </c>
+      <c r="I69" s="109" t="s">
+        <v>31</v>
+      </c>
+      <c r="J69" s="74" t="s">
         <v>87</v>
-      </c>
-      <c r="H69" s="110" t="s">
-        <v>50</v>
-      </c>
-      <c r="I69" s="109" t="s">
-        <v>31</v>
-      </c>
-      <c r="J69" s="74" t="s">
-        <v>88</v>
       </c>
       <c r="K69" s="111" t="s">
         <v>31</v>
@@ -4528,7 +4518,7 @@
     </row>
     <row r="70" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B70" s="112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C70" s="116"/>
       <c r="D70" s="114">
@@ -4537,16 +4527,16 @@
       <c r="E70" s="114"/>
       <c r="F70" s="122"/>
       <c r="G70" s="122" t="s">
+        <v>88</v>
+      </c>
+      <c r="H70" s="116" t="s">
+        <v>49</v>
+      </c>
+      <c r="I70" s="115" t="s">
+        <v>31</v>
+      </c>
+      <c r="J70" s="122" t="s">
         <v>89</v>
-      </c>
-      <c r="H70" s="116" t="s">
-        <v>50</v>
-      </c>
-      <c r="I70" s="115" t="s">
-        <v>31</v>
-      </c>
-      <c r="J70" s="122" t="s">
-        <v>90</v>
       </c>
       <c r="K70" s="117" t="s">
         <v>31</v>
@@ -4561,7 +4551,7 @@
     </row>
     <row r="71" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C71" s="110"/>
       <c r="D71" s="72">
@@ -4570,16 +4560,16 @@
       <c r="E71" s="72"/>
       <c r="F71" s="74"/>
       <c r="G71" s="74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H71" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="I71" s="109" t="s">
+        <v>31</v>
+      </c>
+      <c r="J71" s="74" t="s">
         <v>91</v>
-      </c>
-      <c r="I71" s="109" t="s">
-        <v>31</v>
-      </c>
-      <c r="J71" s="74" t="s">
-        <v>92</v>
       </c>
       <c r="K71" s="111" t="s">
         <v>31</v>
@@ -4594,7 +4584,7 @@
     </row>
     <row r="72" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C72" s="123"/>
       <c r="D72" s="93">
@@ -4603,16 +4593,16 @@
       <c r="E72" s="93"/>
       <c r="F72" s="105"/>
       <c r="G72" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="H72" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="I72" s="124" t="s">
+        <v>31</v>
+      </c>
+      <c r="J72" s="105" t="s">
         <v>93</v>
-      </c>
-      <c r="H72" s="93" t="s">
-        <v>91</v>
-      </c>
-      <c r="I72" s="124" t="s">
-        <v>31</v>
-      </c>
-      <c r="J72" s="105" t="s">
-        <v>94</v>
       </c>
       <c r="K72" s="125" t="s">
         <v>31</v>
@@ -4630,7 +4620,7 @@
       <c r="C73" s="4"/>
       <c r="F73" s="1"/>
       <c r="K73" s="160" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L73" s="161"/>
       <c r="M73" s="162">
@@ -4646,7 +4636,7 @@
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="K75" s="160" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L75" s="161"/>
       <c r="M75" s="162">
@@ -5528,18 +5518,13 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="D8:D10"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="D38:D39"/>
@@ -5547,13 +5532,18 @@
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="B46:B47"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>